<commit_message>
Complete Healthcare_Automation Project Uploaded into Github
</commit_message>
<xml_diff>
--- a/Input_Files/Excel/InputData.xlsx
+++ b/Input_Files/Excel/InputData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="16740" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="45">
   <si>
     <t>browser</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>lenskartCustomer</t>
+  </si>
+  <si>
+    <t>ie</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>a212211</t>
   </si>
 </sst>
 </file>
@@ -477,8 +489,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,39 +514,51 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -546,7 +570,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,6 +631,9 @@
       <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -630,6 +657,9 @@
       <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -652,6 +682,9 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -676,6 +709,9 @@
       <c r="G5" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="H5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -699,6 +735,9 @@
       <c r="G6" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -721,6 +760,9 @@
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -742,13 +784,13 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="75.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -789,13 +831,13 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -832,8 +874,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +896,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
@@ -868,7 +910,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -882,7 +924,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -896,7 +938,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -910,7 +952,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>

</xml_diff>